<commit_message>
Matlab scripts for diagrams
</commit_message>
<xml_diff>
--- a/benchmark/v1.xlsx
+++ b/benchmark/v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gitop\repos\knn-mpi\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59095054-BA60-4F3A-9AD3-551C646A21CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E64109-D776-4C85-AC8E-012B3758CC3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{91893F1A-4A58-4381-A830-40CEDF0CC68C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>corel color histogram</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>miniboone pid</t>
+  </si>
+  <si>
+    <t>bbc</t>
+  </si>
+  <si>
+    <t>cnn</t>
+  </si>
+  <si>
+    <t>cnnibn</t>
+  </si>
+  <si>
+    <t>ndtv</t>
+  </si>
+  <si>
+    <t>timesnow</t>
+  </si>
+  <si>
+    <t>features</t>
   </si>
 </sst>
 </file>
@@ -415,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987B9E06-770E-43A4-8F0C-65ED60A8FE70}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -428,9 +446,10 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="21.54296875" customWidth="1"/>
     <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -446,8 +465,26 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -463,8 +500,26 @@
       <c r="E2">
         <v>238376</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>5319.97</v>
+      </c>
+      <c r="G2">
+        <v>9657.02</v>
+      </c>
+      <c r="H2">
+        <v>18029.900000000001</v>
+      </c>
+      <c r="I2">
+        <v>4969.1400000000003</v>
+      </c>
+      <c r="J2">
+        <v>25186</v>
+      </c>
+      <c r="K2">
+        <v>520072.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -480,8 +535,26 @@
       <c r="E3">
         <v>119897</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>2611.6</v>
+      </c>
+      <c r="G3">
+        <v>4904.2299999999996</v>
+      </c>
+      <c r="H3">
+        <v>9459.1200000000008</v>
+      </c>
+      <c r="I3">
+        <v>2815.15</v>
+      </c>
+      <c r="J3">
+        <v>13141.6</v>
+      </c>
+      <c r="K3">
+        <v>274190.53000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -497,8 +570,26 @@
       <c r="E4">
         <v>60098.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>1731.61</v>
+      </c>
+      <c r="G4">
+        <v>2567.88</v>
+      </c>
+      <c r="H4">
+        <v>5286.9</v>
+      </c>
+      <c r="I4">
+        <v>1587.57</v>
+      </c>
+      <c r="J4">
+        <v>7120.98</v>
+      </c>
+      <c r="K4">
+        <v>154592.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -514,8 +605,26 @@
       <c r="E5">
         <v>37243</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>1099.1300000000001</v>
+      </c>
+      <c r="G5">
+        <v>1508.05</v>
+      </c>
+      <c r="H5">
+        <v>3185.74</v>
+      </c>
+      <c r="I5">
+        <v>977.59699999999998</v>
+      </c>
+      <c r="J5">
+        <v>4229.33</v>
+      </c>
+      <c r="K5">
+        <v>75923.199999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>16</v>
       </c>
@@ -531,8 +640,26 @@
       <c r="E6">
         <v>20216</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>728.529</v>
+      </c>
+      <c r="G6">
+        <v>1057.1099999999999</v>
+      </c>
+      <c r="H6">
+        <v>2030.79</v>
+      </c>
+      <c r="I6">
+        <v>645.07899999999995</v>
+      </c>
+      <c r="J6">
+        <v>2733.85</v>
+      </c>
+      <c r="K6">
+        <v>38885.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>32</v>
       </c>
@@ -549,7 +676,7 @@
         <v>10350.799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>48</v>
       </c>
@@ -566,7 +693,7 @@
         <v>7551.66</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>60</v>
       </c>

</xml_diff>